<commit_message>
Corrección de errores + Cierre [002]
Se corrigen errores en los documentos de evaluación CCB, planificación y pruebas (se cambia el nombre del responsable).
Se incluye la plantilla completada de la actividad de cierre del cambio 002.

Autor: RME_241202
</commit_message>
<xml_diff>
--- a/ControlCambios/03_Evaluacion_CCB/Aceptadas/EvalCCB_002.xlsx
+++ b/ControlCambios/03_Evaluacion_CCB/Aceptadas/EvalCCB_002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romar\Documents\GitHub\EnSo_ControlCambios_gr1.2\ControlCambios\03_Evaluacion_CCB\Aceptadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C3F3BF2-E58C-4FB3-98B0-3ACEDC4A7117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C364CFA-3A17-4FB9-ACE9-58770550DA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5C5BC720-7C65-4E1C-B877-CA64D3505237}"/>
   </bookViews>
@@ -92,12 +92,6 @@
     <t>EvalDes_002</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>john.doe@usc.es</t>
-  </si>
-  <si>
     <t>ACEPTADO</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>Se decide aprobar el cambio teniendo en cuenta su buena relación entre la factibilidad, dificultad y valor que aporta a la aplicación. Se asigna una prioridad media al no tratarse de un hecho crítico para la existencia de la aplicación, pero sí se valora su gran utilidad para sus usuarios.</t>
+  </si>
+  <si>
+    <t>Roi Martínez Enríquez</t>
+  </si>
+  <si>
+    <t>roi.martinez.enriquez@rai.usc.es</t>
   </si>
 </sst>
 </file>
@@ -540,6 +540,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -577,33 +604,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -924,7 +924,7 @@
   <dimension ref="C2:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,24 +949,24 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="45" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="31"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
@@ -979,12 +979,12 @@
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
-      <c r="F7" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="F7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
@@ -993,12 +993,12 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="F8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
@@ -1007,12 +1007,12 @@
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
@@ -1021,12 +1021,12 @@
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1041,10 +1041,10 @@
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="42"/>
+      <c r="D12" s="31"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
@@ -1058,7 +1058,7 @@
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
@@ -1078,7 +1078,7 @@
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
       <c r="F16" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
@@ -1105,45 +1105,45 @@
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="8"/>
-      <c r="D19" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
+      <c r="D19" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="8"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="31"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="40"/>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="8"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="8"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="16"/>
@@ -1156,24 +1156,30 @@
       <c r="J23" s="18"/>
     </row>
     <row r="24" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37" t="s">
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="38"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="P31" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="D19:J22"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="I24:J24"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="C4:F4"/>
@@ -1188,12 +1194,6 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="D19:J22"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="I24:J24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{279FB9B5-0976-48F5-A886-E06515C3767F}"/>

</xml_diff>